<commit_message>
Added Nations Trust coming soon
</commit_message>
<xml_diff>
--- a/scraper/Card Deals/Reference/Results_summary.xlsx
+++ b/scraper/Card Deals/Reference/Results_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AI Projects\LLM Web App\firstproject\FD rates 2\my-fd-comparison\scraper\Card Deals\Reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B19818-67A8-495D-B5DF-4D15A36FAC67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52049FC5-4E81-428D-A213-BEBE79F008E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{63884344-BE03-4277-AB84-50C111B02458}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -36,7 +36,22 @@
     <t>Combank</t>
   </si>
   <si>
-    <t>Getting few null values for merchant details. Extracting it from promo title</t>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Getting few null values for merchant details for general promos. Extracting it from promo title</t>
+  </si>
+  <si>
+    <t>DFCC</t>
+  </si>
+  <si>
+    <t>HNB</t>
+  </si>
+  <si>
+    <t>In promo details check how to make the main field (text before :) to bold like in the website</t>
+  </si>
+  <si>
+    <t>NDB</t>
   </si>
 </sst>
 </file>
@@ -388,32 +403,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D2F4877-844D-4655-B7F7-D8BE5B726F5E}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
-    <col min="2" max="2" width="31" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="3" max="3" width="68.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added last updated and run all scrapers script
</commit_message>
<xml_diff>
--- a/scraper/Card Deals/Reference/Results_summary.xlsx
+++ b/scraper/Card Deals/Reference/Results_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AI Projects\LLM Web App\firstproject\FD rates 2\my-fd-comparison\scraper\Card Deals\Reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D094E686-067C-403B-854C-AC68FC1A5342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C87FE2-0783-42A4-9417-20FB6B285BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{63884344-BE03-4277-AB84-50C111B02458}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -76,14 +76,37 @@
   </si>
   <si>
     <t>Didn’t take merchant name of first two promos in each category</t>
+  </si>
+  <si>
+    <t>People Bank</t>
+  </si>
+  <si>
+    <t>Sampath</t>
+  </si>
+  <si>
+    <t>Seylan</t>
+  </si>
+  <si>
+    <t>Need to give proper summary in console</t>
+  </si>
+  <si>
+    <t>Feb 4th run</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -111,9 +134,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,34 +452,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D2F4877-844D-4655-B7F7-D8BE5B726F5E}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" customWidth="1"/>
-    <col min="2" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="68.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="23.140625" customWidth="1"/>
+    <col min="5" max="5" width="68.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -463,73 +490,122 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
       <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
       <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>